<commit_message>
added the ability to take screenshots
</commit_message>
<xml_diff>
--- a/_test-output/excel.xlsx
+++ b/_test-output/excel.xlsx
@@ -11,10 +11,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Protractor results for: 2016-11-02 17:03:24
+    <t>Protractor results for: 2016-11-03 17:21:17
 </t>
+  </si>
+  <si>
+    <t>AppDir:./</t>
+  </si>
+  <si>
+    <t>Suite:</t>
+  </si>
+  <si>
+    <t>QuickStart E2E Tests</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>should open index page</t>
+  </si>
+  <si>
+    <t>should display app.component heading</t>
   </si>
 </sst>
 </file>
@@ -46,8 +64,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyFont="1" fontId="0"/>
+    <xf applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -55,7 +76,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr/>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -69,6 +90,38 @@
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
     </row>
+    <row r="2" spans="2:2">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4">
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="5:5">
+      <c r="B5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>